<commit_message>
Merged sistema-automatico-de-pausa-a-fin-de-dia into master
</commit_message>
<xml_diff>
--- a/data/production_data.xlsx
+++ b/data/production_data.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T92"/>
+  <dimension ref="A1:T101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
@@ -5448,7 +5448,7 @@
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>en proceso</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="L64" t="n">
@@ -5474,6 +5474,11 @@
           <t>2024-07-08 23:02</t>
         </is>
       </c>
+      <c r="T64" t="inlineStr">
+        <is>
+          <t>2024-07-12 16:48</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -5750,7 +5755,7 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>en proceso</t>
+          <t>Paused</t>
         </is>
       </c>
       <c r="L68" t="n">
@@ -5761,6 +5766,16 @@
           <t>L1</t>
         </is>
       </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>2024-07-13 15:56</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>Fin del día automático</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -5813,7 +5828,7 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>en proceso</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="L69" t="n">
@@ -5824,6 +5839,26 @@
           <t>L1</t>
         </is>
       </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>2024-07-12 07:51</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>Fin del día</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>2024-07-12 07:51</t>
+        </is>
+      </c>
+      <c r="T69" t="inlineStr">
+        <is>
+          <t>2024-07-12 09:02</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -5949,7 +5984,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>en proceso</t>
+          <t>Paused</t>
         </is>
       </c>
       <c r="L71" t="n">
@@ -5960,6 +5995,16 @@
           <t>L2</t>
         </is>
       </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>2024-07-13 15:56</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>Fin del día automático</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -6362,7 +6407,7 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>en proceso</t>
+          <t>Paused</t>
         </is>
       </c>
       <c r="L77" t="n">
@@ -6373,6 +6418,16 @@
           <t>L1</t>
         </is>
       </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>2024-07-13 15:56</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>Fin del día automático</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -6498,7 +6553,7 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Paused</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="L79" t="n">
@@ -6519,6 +6574,26 @@
           <t>Pausa para almorzar</t>
         </is>
       </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>2024-07-12 12:51</t>
+        </is>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>2024-07-12 12:52</t>
+        </is>
+      </c>
+      <c r="R79" t="inlineStr">
+        <is>
+          <t>Falta de materiales: Corrugado</t>
+        </is>
+      </c>
+      <c r="T79" t="inlineStr">
+        <is>
+          <t>2024-07-12 12:52</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -6592,6 +6667,21 @@
           <t>Pausa para almorzar</t>
         </is>
       </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>2024-07-13 15:56</t>
+        </is>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>2024-07-13 15:57</t>
+        </is>
+      </c>
+      <c r="R80" t="inlineStr">
+        <is>
+          <t>Fin del día automático</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -6644,7 +6734,7 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>en proceso</t>
+          <t>Paused</t>
         </is>
       </c>
       <c r="L81" t="n">
@@ -6655,6 +6745,16 @@
           <t>L1</t>
         </is>
       </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>2024-07-13 15:56</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Fin del día automático</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -6707,7 +6807,7 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>en proceso</t>
+          <t>Paused</t>
         </is>
       </c>
       <c r="L82" t="n">
@@ -6718,6 +6818,16 @@
           <t>L1</t>
         </is>
       </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>2024-07-13 15:56</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Fin del día automático</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -6770,7 +6880,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>en proceso</t>
+          <t>Paused</t>
         </is>
       </c>
       <c r="L83" t="n">
@@ -6781,6 +6891,16 @@
           <t>L1</t>
         </is>
       </c>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>2024-07-13 15:56</t>
+        </is>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>Fin del día automático</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -6833,7 +6953,7 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>en proceso</t>
+          <t>Paused</t>
         </is>
       </c>
       <c r="L84" t="n">
@@ -6844,6 +6964,16 @@
           <t>L1</t>
         </is>
       </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>2024-07-13 15:56</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Fin del día automático</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -6974,7 +7104,7 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>en proceso</t>
+          <t>Paused</t>
         </is>
       </c>
       <c r="L86" t="n">
@@ -6985,6 +7115,16 @@
           <t>L1</t>
         </is>
       </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>2024-07-12 07:52</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>Pausa para almorzar</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -7105,7 +7245,7 @@
       </c>
       <c r="K88" t="inlineStr">
         <is>
-          <t>en proceso</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="L88" t="n">
@@ -7116,6 +7256,11 @@
           <t>L1</t>
         </is>
       </c>
+      <c r="T88" t="inlineStr">
+        <is>
+          <t>2024-07-12 07:50</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -7319,7 +7464,7 @@
       </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>en proceso</t>
+          <t>Paused</t>
         </is>
       </c>
       <c r="L91" t="n">
@@ -7330,6 +7475,16 @@
           <t>L1</t>
         </is>
       </c>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>2024-07-13 15:56</t>
+        </is>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>Fin del día automático</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -7382,7 +7537,7 @@
       </c>
       <c r="K92" t="inlineStr">
         <is>
-          <t>en proceso</t>
+          <t>Paused</t>
         </is>
       </c>
       <c r="L92" t="n">
@@ -7393,13 +7548,648 @@
           <t>L1</t>
         </is>
       </c>
-      <c r="N92" t="inlineStr"/>
-      <c r="O92" t="inlineStr"/>
-      <c r="P92" t="inlineStr"/>
-      <c r="Q92" t="inlineStr"/>
-      <c r="R92" t="inlineStr"/>
-      <c r="S92" t="inlineStr"/>
-      <c r="T92" t="inlineStr"/>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>2024-07-12 12:51</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>Pausa para almorzar</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>8218092e-4e36-4b61-960c-0e971b07466b</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>2024-07-12 07:50</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>9</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>FRANCISCO DIAZ</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Walfred Lira</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>ELECTRICIDAD</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Bosquemar</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>Iluminación</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>Paused</t>
+        </is>
+      </c>
+      <c r="L93" t="n">
+        <v>4</v>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>2024-07-13 15:56</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>Fin del día automático</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>76292e9b-9f21-40d4-bbf0-669d245975c2</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>2024-07-12 07:53</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>7</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>CESAR VILLARROEL</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Luis Recabal</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>CARPINTERIA</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Puyaral</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>Barrera de humedad Volcanwrap exterior muros</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="L94" t="n">
+        <v>4</v>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="T94" t="inlineStr">
+        <is>
+          <t>2024-07-12 07:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>d887c85e-f175-4bd4-aa3b-76cf773a7244</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>2024-07-12 08:57</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>7</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>CESAR VILLARROEL</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Luis Recabal</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>CARPINTERIA</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Puyaral</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>Piso SPC</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="L95" t="n">
+        <v>4</v>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="T95" t="inlineStr">
+        <is>
+          <t>2024-07-12 08:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>f151ce73-54b7-46ae-b271-7a5dd9b9aefe</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>2024-07-12 12:39</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>35</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>FRANCISCO DIAZ</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>CLAUDIO ROJAS</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>PINTURA</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Puyaral</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>Pintura Interior (2° mano)</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>Paused</t>
+        </is>
+      </c>
+      <c r="L96" t="n">
+        <v>1</v>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>2024-07-12 12:39</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>Fin del día</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>efcab23b-415e-4d2a-aadf-1f62c0d44829</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>2024-07-12 13:03</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>25</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>CESAR VILLARROEL</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Celso Martinez</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>CARPINTERIA</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Las Bandurrias</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>Instalación OSB</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="L97" t="n">
+        <v>4</v>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>L2</t>
+        </is>
+      </c>
+      <c r="T97" t="inlineStr">
+        <is>
+          <t>2024-07-12 13:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>73fb3577-6673-4829-a8a6-5fb9e019701a</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>2024-07-12 13:15</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>25</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>CESAR VILLARROEL</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Celso Martinez</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>CARPINTERIA</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Puyaral</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>Guardapolvos y pilastras</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>Paused</t>
+        </is>
+      </c>
+      <c r="L98" t="n">
+        <v>4</v>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>L2</t>
+        </is>
+      </c>
+      <c r="N98" t="inlineStr">
+        <is>
+          <t>2024-07-12 16:28</t>
+        </is>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>Fin del día</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>95888789-eb8c-483e-9456-6a5677581cba</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>2024-07-12 16:15</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>39</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>FRANCISCO DIAZ</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>DIEGO RIOSECO</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>GASFITERÍA</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Las Bandurrias</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>Artefactos sanitarios</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>Paused</t>
+        </is>
+      </c>
+      <c r="L99" t="n">
+        <v>3</v>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>L2</t>
+        </is>
+      </c>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>2024-07-12 16:16</t>
+        </is>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>Fin del día</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>9c10e9aa-0664-48e2-af1f-77c612e2646e</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>2024-07-12 16:46</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>25</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>CESAR VILLARROEL</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>CELSO MARTINEZ</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>CARPINTERIA</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Las Bandurrias</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>Instalación Escalera</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="L100" t="n">
+        <v>3</v>
+      </c>
+      <c r="M100" t="inlineStr">
+        <is>
+          <t>L2</t>
+        </is>
+      </c>
+      <c r="T100" t="inlineStr">
+        <is>
+          <t>2024-07-12 16:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2433e744-e529-44df-914e-921d5cd4fa25</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>2024-07-12 16:53</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>46</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>CAMILO CASTILLO</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>ABRAHAM BECERRA</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>PINTURA</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>Las Bandurrias</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>Pintura Interior (2° mano)</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="L101" t="n">
+        <v>3</v>
+      </c>
+      <c r="M101" t="inlineStr">
+        <is>
+          <t>L2</t>
+        </is>
+      </c>
+      <c r="T101" t="inlineStr">
+        <is>
+          <t>2024-07-12 16:53</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
cleaner base.html, removed all fullscreen.js traces
</commit_message>
<xml_diff>
--- a/data/production_data.xlsx
+++ b/data/production_data.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T101"/>
+  <dimension ref="A1:T110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
@@ -5209,7 +5209,7 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Paused</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="L61" t="n">
@@ -5245,6 +5245,11 @@
           <t>Pausa para almorzar</t>
         </is>
       </c>
+      <c r="T61" t="inlineStr">
+        <is>
+          <t>2024-07-15 00:20</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -5755,7 +5760,7 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>Paused</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="L68" t="n">
@@ -5776,6 +5781,11 @@
           <t>Fin del día automático</t>
         </is>
       </c>
+      <c r="T68" t="inlineStr">
+        <is>
+          <t>2024-07-15 00:20</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -6953,7 +6963,7 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>Paused</t>
+          <t>Finished</t>
         </is>
       </c>
       <c r="L84" t="n">
@@ -6974,6 +6984,11 @@
           <t>Fin del día automático</t>
         </is>
       </c>
+      <c r="T84" t="inlineStr">
+        <is>
+          <t>2024-07-15 00:57</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -8188,6 +8203,613 @@
       <c r="T101" t="inlineStr">
         <is>
           <t>2024-07-12 16:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>ec7bec93-68de-45e3-a277-503428236ec5</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>2024-07-15 00:20</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>32</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>CESAR VILLARROEL</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Carlos Astorga</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>CARPINTERIA</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>Puyaral</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>Guardapolvos y pilastras</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="L102" t="n">
+        <v>1</v>
+      </c>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="T102" t="inlineStr">
+        <is>
+          <t>2024-07-15 00:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>06b0cafd-b600-4510-a1af-156aadf6f614</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>2024-07-15 00:20</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>32</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>CESAR VILLARROEL</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Carlos Astorga</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>CARPINTERIA</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Puyaral</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>Instalación OSB</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="L103" t="n">
+        <v>1</v>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="T103" t="inlineStr">
+        <is>
+          <t>2024-07-15 00:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>8892e157-d06e-4ad5-94f7-288555094449</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>2024-07-15 00:20</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>32</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>CESAR VILLARROEL</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Carlos Astorga</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>CARPINTERIA</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Puyaral</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>Instalación OSB</t>
+        </is>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="L104" t="n">
+        <v>1</v>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="T104" t="inlineStr">
+        <is>
+          <t>2024-07-15 00:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>a2ef94a5-c02a-4c49-b85c-7787d9182cd6</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>2024-07-15 00:21</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>32</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>CESAR VILLARROEL</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Carlos Astorga</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>CARPINTERIA</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Puyaral</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>Instalación OSB</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="L105" t="n">
+        <v>1</v>
+      </c>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="T105" t="inlineStr">
+        <is>
+          <t>2024-07-15 00:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>b0e9d0ae-e261-4ba4-be9f-813fa269b1a6</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>2024-07-15 00:21</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>32</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>CESAR VILLARROEL</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Carlos Astorga</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>CARPINTERIA</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>Puyaral</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>Instalación OSB</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>en proceso</t>
+        </is>
+      </c>
+      <c r="L106" t="n">
+        <v>1</v>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>ac8b686b-652e-41cd-912a-be7752f2f374</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>2024-07-15 00:58</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>12</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>FRANCISCO DIAZ</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Flor Sanhueza</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>SELLOS Y ASEO</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>Puyaral</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>Aseo entrega</t>
+        </is>
+      </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>Paused</t>
+        </is>
+      </c>
+      <c r="L107" t="n">
+        <v>1</v>
+      </c>
+      <c r="M107" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t>2024-07-15 00:59</t>
+        </is>
+      </c>
+      <c r="O107" t="inlineStr">
+        <is>
+          <t>Final del día</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>3c1e37fd-6866-4c4e-b4df-fdf3aa9e9c1c</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>2024-07-15 09:08</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>25</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>CESAR VILLARROEL</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>CELSO MARTINEZ</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>CARPINTERIA</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>Las Bandurrias</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>Instalación de puerta interior</t>
+        </is>
+      </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="L108" t="n">
+        <v>1</v>
+      </c>
+      <c r="M108" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="T108" t="inlineStr">
+        <is>
+          <t>2024-07-15 09:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>240f279e-469b-45fd-b098-cdcbc15480b9</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>2024-07-15 09:08</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>25</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>CESAR VILLARROEL</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Celso Martinez</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>CARPINTERIA</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>Las Bandurrias</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>Revestimiento Siding (planchas)</t>
+        </is>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>en proceso</t>
+        </is>
+      </c>
+      <c r="L109" t="n">
+        <v>1</v>
+      </c>
+      <c r="M109" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>a2a02727-8a93-43a4-a62c-8f836eb05283</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>2024-07-15 09:09</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>12</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>FRANCISCO DIAZ</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>FLOR SANHUEZA</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>SELLOS Y ASEO</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>Bosquemar</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>Aseo entrega</t>
+        </is>
+      </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>Finished</t>
+        </is>
+      </c>
+      <c r="L110" t="n">
+        <v>4</v>
+      </c>
+      <c r="M110" t="inlineStr">
+        <is>
+          <t>L2</t>
+        </is>
+      </c>
+      <c r="T110" t="inlineStr">
+        <is>
+          <t>2024-07-15 09:09</t>
         </is>
       </c>
     </row>

</xml_diff>